<commit_message>
added top 3 experiment
</commit_message>
<xml_diff>
--- a/results-report-template.xlsx
+++ b/results-report-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Semester2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE49CD75-DF42-48E5-9F23-622B9FC69E18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBFD535-214A-4CFD-9503-6CE7A6441BA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="990" windowWidth="21600" windowHeight="11340" xr2:uid="{FF84E361-6D82-4BEC-B641-EB19EF216FBF}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,13 +440,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="C2">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="D2">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="E2">
         <v>1367</v>
@@ -457,13 +457,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>0.54</v>
       </c>
       <c r="C3">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="D3">
-        <v>0.56999999999999995</v>
+        <v>0.59</v>
       </c>
       <c r="E3">
         <v>1194</v>
@@ -474,13 +474,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="C4">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="E4">
         <v>1193</v>
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.37</v>
+        <v>0.38</v>
       </c>
       <c r="C5">
-        <v>0.23</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D5">
-        <v>0.28000000000000003</v>
+        <v>0.33</v>
       </c>
       <c r="E5">
         <v>650</v>
@@ -508,13 +508,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="C6">
-        <v>0.25</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D6">
-        <v>0.28000000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E6">
         <v>519</v>
@@ -525,13 +525,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.33</v>
+        <v>0.39</v>
       </c>
       <c r="C7">
-        <v>0.13</v>
+        <v>0.23</v>
       </c>
       <c r="D7">
-        <v>0.19</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E7">
         <v>326</v>
@@ -542,13 +542,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.38</v>
+        <v>0.47</v>
       </c>
       <c r="C8">
-        <v>0.22</v>
+        <v>0.27</v>
       </c>
       <c r="D8">
-        <v>0.28000000000000003</v>
+        <v>0.35</v>
       </c>
       <c r="E8">
         <v>343</v>
@@ -559,13 +559,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.49</v>
+        <v>0.54</v>
       </c>
       <c r="C9">
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
       <c r="D9">
-        <v>0.19</v>
+        <v>0.25</v>
       </c>
       <c r="E9">
         <v>314</v>
@@ -576,13 +576,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.36</v>
+        <v>0.41</v>
       </c>
       <c r="C10">
-        <v>0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D10">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
       <c r="E10">
         <v>307</v>
@@ -593,13 +593,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="C11">
-        <v>0.21</v>
+        <v>0.31</v>
       </c>
       <c r="D11">
-        <v>0.28000000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="E11">
         <v>326</v>
@@ -610,13 +610,13 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="C12">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="D12">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="E12">
         <v>6539</v>
@@ -627,13 +627,13 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="C13">
-        <v>0.31</v>
+        <v>0.36</v>
       </c>
       <c r="D13">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="E13">
         <v>6539</v>
@@ -644,13 +644,13 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>0.41</v>
+        <v>0.44</v>
       </c>
       <c r="C14">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="D14">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="E14">
         <v>6539</v>

</xml_diff>